<commit_message>
Plans et data movement
</commit_message>
<xml_diff>
--- a/02_Commandes/Commande_P1704_2019.xlsx
+++ b/02_Commandes/Commande_P1704_2019.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Exemple" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -85,6 +85,51 @@
   </si>
   <si>
     <t>https://www.digikey.ch/product-detail/fr/nkk-switches/AT9704-085L/360-2346-ND/2039173?cur=CHF&amp;lang=fr</t>
+  </si>
+  <si>
+    <t>Contact LED rouge/vert</t>
+  </si>
+  <si>
+    <t>679-2256-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/product-detail/fr/mec-switches/4FTH98222/679-2256-ND/2034812</t>
+  </si>
+  <si>
+    <t>Contact LED bleue</t>
+  </si>
+  <si>
+    <t>679-2251-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/product-detail/fr/mec-switches/4FTH901/679-2251-ND/2034807?cur=CHF&amp;lang=fr</t>
+  </si>
+  <si>
+    <t>Contact LED jaune</t>
+  </si>
+  <si>
+    <t>679-2253-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/product-detail/fr/mec-switches/4FTH942/679-2253-ND/2034809</t>
+  </si>
+  <si>
+    <t>Capuchon triangulaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  679-2129-ND </t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/product-detail/fr/mec-switches/1V16/679-2129-ND/2034685</t>
+  </si>
+  <si>
+    <t>Capuchon cercle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">679-2125-ND </t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/product-detail/fr/mec-switches/1U16/679-2125-ND/2034681</t>
   </si>
 </sst>
 </file>
@@ -135,7 +180,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -150,6 +195,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -204,8 +250,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:I5" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A1:I5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:I9" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:I9"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Date" dataDxfId="8"/>
     <tableColumn id="2" name="Quantité" dataDxfId="7"/>
@@ -511,7 +557,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,15 +684,150 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="K5" s="5"/>
+      <c r="A5" s="4">
+        <v>43545</v>
+      </c>
+      <c r="B5" s="1">
+        <v>15</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="1">
+        <v>5.62</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>43545</v>
+      </c>
+      <c r="B6" s="1">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="1">
+        <v>7.76</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>43545</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="1">
+        <v>4.59</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>43545</v>
+      </c>
+      <c r="B8" s="1">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>43545</v>
+      </c>
+      <c r="B9" s="1">
+        <v>12</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.62</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="10" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -668,11 +849,16 @@
     <hyperlink ref="K2" r:id="rId1"/>
     <hyperlink ref="K3" r:id="rId2"/>
     <hyperlink ref="K4" r:id="rId3"/>
+    <hyperlink ref="K7" r:id="rId4"/>
+    <hyperlink ref="K6" r:id="rId5"/>
+    <hyperlink ref="K8" r:id="rId6"/>
+    <hyperlink ref="K9" r:id="rId7"/>
+    <hyperlink ref="K5" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>